<commit_message>
orderforn lob and tier implement
orderforn lob and tier implement
</commit_message>
<xml_diff>
--- a/public/template/sample_template.xlsx
+++ b/public/template/sample_template.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SVN-SHR\beta\public\template\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Automation.PC-SHR-0074\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE788CC8-B148-442D-9368-3A899E925088}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E595815-C7B0-48C0-9593-DBCB5D6837CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="15000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="23">
   <si>
     <t>Order Received Data and Time</t>
   </si>
@@ -62,9 +62,6 @@
     <t>Status</t>
   </si>
   <si>
-    <t>SIPL0003</t>
-  </si>
-  <si>
     <t>SIPL0004</t>
   </si>
   <si>
@@ -80,13 +77,34 @@
     <t>WIP</t>
   </si>
   <si>
-    <t>Broker Support</t>
-  </si>
-  <si>
-    <t>Loan Registration</t>
-  </si>
-  <si>
-    <t>Completed</t>
+    <t>Product Type</t>
+  </si>
+  <si>
+    <t>Tier</t>
+  </si>
+  <si>
+    <t>Lob</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Search(T1) </t>
+  </si>
+  <si>
+    <t>Appraisal</t>
+  </si>
+  <si>
+    <t>Servicing</t>
+  </si>
+  <si>
+    <t>Two Owner</t>
+  </si>
+  <si>
+    <t>2 Owner - PIR</t>
+  </si>
+  <si>
+    <t>Search(T2)</t>
+  </si>
+  <si>
+    <t>SIPL0005</t>
   </si>
 </sst>
 </file>
@@ -600,7 +618,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
@@ -608,7 +626,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="42">
@@ -965,23 +982,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H4"/>
+  <dimension ref="A1:K3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="28.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="36.28515625" customWidth="1"/>
     <col min="4" max="4" width="12.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="16" customWidth="1"/>
     <col min="8" max="8" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.85546875" customWidth="1"/>
+    <col min="10" max="10" width="24.5703125" customWidth="1"/>
+    <col min="11" max="11" width="11.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -1006,79 +1026,84 @@
       <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
+      <c r="I1" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>14</v>
+      </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="6">
-        <v>45587</v>
+    <row r="2" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="5">
+        <v>45436</v>
       </c>
       <c r="B2" s="2">
-        <v>5246</v>
+        <v>134425</v>
       </c>
       <c r="C2" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D2" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="E2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="F2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="G2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="H2" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="H2" s="2" t="s">
-        <v>13</v>
+      <c r="I2" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="6">
-        <v>45588</v>
+    <row r="3" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="5">
+        <v>45439</v>
       </c>
       <c r="B3" s="2">
-        <v>9744</v>
+        <v>359925</v>
       </c>
       <c r="C3" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D3" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="E3" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="E3" s="2" t="s">
-        <v>14</v>
-      </c>
       <c r="F3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G3" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="G3" s="2" t="s">
+      <c r="H3" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="H3" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="6">
-        <v>45589</v>
-      </c>
-      <c r="B4" s="2">
-        <v>3345</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="F4" s="2"/>
-      <c r="G4" s="2"/>
-      <c r="H4" s="2" t="s">
-        <v>16</v>
+      <c r="I3" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="K3" s="2" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
excel upload changes 07/03/2024
excel upload changes 07/03/2024
</commit_message>
<xml_diff>
--- a/public/template/sample_template.xlsx
+++ b/public/template/sample_template.xlsx
@@ -2,20 +2,20 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
-  <workbookPr defaultThemeVersion="202300"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Automation\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Automation.PC-SHR-0074\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5E3D3589-D86A-43F0-8A19-24F8BBA3C0AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97F21CA7-9D4B-48E4-9491-3D1C12123747}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{92448108-0D2B-4F64-825C-424C9CF81D68}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="15000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="with_all_correctdata" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="18">
   <si>
     <t>Order Received Data and Time</t>
   </si>
@@ -50,9 +50,6 @@
     <t>Assignee_QA</t>
   </si>
   <si>
-    <t>Product Name</t>
-  </si>
-  <si>
     <t>State</t>
   </si>
   <si>
@@ -62,28 +59,37 @@
     <t>Status</t>
   </si>
   <si>
+    <t>SIPL0004</t>
+  </si>
+  <si>
+    <t>FL</t>
+  </si>
+  <si>
+    <t>Clay</t>
+  </si>
+  <si>
+    <t>WIP</t>
+  </si>
+  <si>
     <t>Tier</t>
   </si>
   <si>
-    <t>SIPL5141</t>
-  </si>
-  <si>
-    <t>1 Owner - FCL Info</t>
-  </si>
-  <si>
-    <t>FL</t>
-  </si>
-  <si>
-    <t>Clay</t>
-  </si>
-  <si>
-    <t>WIP</t>
-  </si>
-  <si>
     <t xml:space="preserve">Search(T1) </t>
   </si>
   <si>
     <t>Search(T2)</t>
+  </si>
+  <si>
+    <t>SIPL0005</t>
+  </si>
+  <si>
+    <t>SPID-007-03</t>
+  </si>
+  <si>
+    <t>SPID-007-32</t>
+  </si>
+  <si>
+    <t>Product Code</t>
   </si>
 </sst>
 </file>
@@ -93,35 +99,327 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-409]m/d/yy\ h:mm\ AM/PM;@"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
-      <scheme val="minor"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri Light"/>
+      <family val="2"/>
+      <scheme val="major"/>
     </font>
     <font>
       <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C5700"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Aptos Narrow"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="8"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <family val="2"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -129,19 +427,120 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="3">
+  <borders count="11">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -159,36 +558,100 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="42">
+    <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
+    <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="20% - Accent4" xfId="31" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="20% - Accent5" xfId="35" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="20% - Accent6" xfId="39" builtinId="50" customBuiltin="1"/>
+    <cellStyle name="40% - Accent1" xfId="20" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="40% - Accent2" xfId="24" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="40% - Accent3" xfId="28" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="40% - Accent4" xfId="32" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="40% - Accent5" xfId="36" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="40% - Accent6" xfId="40" builtinId="51" customBuiltin="1"/>
+    <cellStyle name="60% - Accent1" xfId="21" builtinId="32" customBuiltin="1"/>
+    <cellStyle name="60% - Accent2" xfId="25" builtinId="36" customBuiltin="1"/>
+    <cellStyle name="60% - Accent3" xfId="29" builtinId="40" customBuiltin="1"/>
+    <cellStyle name="60% - Accent4" xfId="33" builtinId="44" customBuiltin="1"/>
+    <cellStyle name="60% - Accent5" xfId="37" builtinId="48" customBuiltin="1"/>
+    <cellStyle name="60% - Accent6" xfId="41" builtinId="52" customBuiltin="1"/>
+    <cellStyle name="Accent1" xfId="18" builtinId="29" customBuiltin="1"/>
+    <cellStyle name="Accent2" xfId="22" builtinId="33" customBuiltin="1"/>
+    <cellStyle name="Accent3" xfId="26" builtinId="37" customBuiltin="1"/>
+    <cellStyle name="Accent4" xfId="30" builtinId="41" customBuiltin="1"/>
+    <cellStyle name="Accent5" xfId="34" builtinId="45" customBuiltin="1"/>
+    <cellStyle name="Accent6" xfId="38" builtinId="49" customBuiltin="1"/>
+    <cellStyle name="Bad" xfId="7" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="Calculation" xfId="11" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="Check Cell" xfId="13" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="Explanatory Text" xfId="16" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
+    <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="1"/>
+    <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
+    <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -204,9 +667,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -214,39 +677,39 @@
         <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="0E2841"/>
+        <a:srgbClr val="44546A"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="E8E8E8"/>
+        <a:srgbClr val="E7E6E6"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="156082"/>
+        <a:srgbClr val="4472C4"/>
       </a:accent1>
       <a:accent2>
-        <a:srgbClr val="E97132"/>
+        <a:srgbClr val="ED7D31"/>
       </a:accent2>
       <a:accent3>
-        <a:srgbClr val="196B24"/>
+        <a:srgbClr val="A5A5A5"/>
       </a:accent3>
       <a:accent4>
-        <a:srgbClr val="0F9ED5"/>
+        <a:srgbClr val="FFC000"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="A02B93"/>
+        <a:srgbClr val="5B9BD5"/>
       </a:accent5>
       <a:accent6>
-        <a:srgbClr val="4EA72E"/>
+        <a:srgbClr val="70AD47"/>
       </a:accent6>
       <a:hlink>
-        <a:srgbClr val="467886"/>
+        <a:srgbClr val="0563C1"/>
       </a:hlink>
       <a:folHlink>
-        <a:srgbClr val="96607D"/>
+        <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
-        <a:latin typeface="Aptos Display" panose="02110004020202020204"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -298,7 +761,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Aptos Narrow" panose="02110004020202020204"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -350,7 +813,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -409,6 +872,13 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
         <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
@@ -417,13 +887,6 @@
           <a:miter lim="800000"/>
         </a:ln>
         <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -488,141 +951,124 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
-  <a:objectDefaults>
-    <a:lnDef>
-      <a:spPr/>
-      <a:bodyPr/>
-      <a:lstStyle/>
-      <a:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </a:style>
-    </a:lnDef>
-  </a:objectDefaults>
+  <a:objectDefaults/>
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{2E142A2C-CD16-42D6-873A-C26D2A0506FA}" vid="{1BDDFF52-6CD6-40A5-AB3C-68EB2F1E4D0A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E10B7538-2170-4379-AF23-D71FA73EA9BC}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.1796875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.26953125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.08984375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.453125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.6328125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="5.1796875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="6.81640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="6.1796875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="28.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="36.28515625" customWidth="1"/>
+    <col min="4" max="4" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16" customWidth="1"/>
+    <col min="8" max="8" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="F1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="2">
+        <v>45436</v>
+      </c>
+      <c r="B2" s="1">
+        <v>1213218873</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="E2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2" s="1" t="s">
         <v>8</v>
       </c>
+      <c r="G2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>12</v>
+      </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A2" s="3">
-        <v>45436</v>
-      </c>
-      <c r="B2" s="4">
-        <v>2001</v>
-      </c>
-      <c r="C2" s="4" t="s">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="2">
+        <v>45439</v>
+      </c>
+      <c r="B3" s="1">
+        <v>21932183821</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G3" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="4"/>
-      <c r="E2" s="5" t="s">
+      <c r="H3" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="F2" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="G2" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="H2" s="4" t="s">
+      <c r="I3" s="1" t="s">
         <v>13</v>
-      </c>
-      <c r="I2" s="4" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A3" s="3">
-        <v>45441.916666666664</v>
-      </c>
-      <c r="B3" s="4">
-        <v>2002</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D3" s="4"/>
-      <c r="E3" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="F3" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="G3" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="H3" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="I3" s="4" t="s">
-        <v>15</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="18" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
new client Accurate added
new client Accurate added on 09/04/2024
</commit_message>
<xml_diff>
--- a/public/template/sample_template.xlsx
+++ b/public/template/sample_template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Automation\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\stellar-oms(dev)\public\template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BBB360E-88B0-4B21-A71E-8C31B1FC2C77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{349603B1-4D78-42D6-B582-5F50786D3463}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="with_all_correctdata" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="24">
   <si>
     <t>Order Received Data and Time</t>
   </si>
@@ -96,6 +96,18 @@
   </si>
   <si>
     <t>Servicing</t>
+  </si>
+  <si>
+    <t>Typist</t>
+  </si>
+  <si>
+    <t>Typist QC</t>
+  </si>
+  <si>
+    <t>SIPL0102</t>
+  </si>
+  <si>
+    <t>SIPL0103</t>
   </si>
 </sst>
 </file>
@@ -969,24 +981,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J3"/>
+  <dimension ref="A1:L3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="L12" sqref="L12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="28.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="28.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="36.28515625" customWidth="1"/>
-    <col min="4" max="4" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="36.33203125" customWidth="1"/>
+    <col min="4" max="4" width="12.6640625" bestFit="1" customWidth="1"/>
     <col min="5" max="6" width="16" customWidth="1"/>
-    <col min="9" max="9" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.5703125" customWidth="1"/>
+    <col min="9" max="9" width="10.88671875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1017,8 +1029,14 @@
       <c r="J1" s="3" t="s">
         <v>11</v>
       </c>
+      <c r="K1" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>21</v>
+      </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2" s="2">
         <v>45436</v>
       </c>
@@ -1049,8 +1067,14 @@
       <c r="J2" s="1" t="s">
         <v>12</v>
       </c>
+      <c r="K2" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>23</v>
+      </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
         <v>45439</v>
       </c>
@@ -1080,6 +1104,12 @@
       </c>
       <c r="J3" s="1" t="s">
         <v>13</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>